<commit_message>
- lots of heuristics added
</commit_message>
<xml_diff>
--- a/heuristics.xlsx
+++ b/heuristics.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" tabRatio="841" activeTab="5"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" tabRatio="841" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="rules" sheetId="8" r:id="rId1"/>
@@ -18,13 +18,14 @@
     <sheet name="direct address to someone" sheetId="4" r:id="rId9"/>
     <sheet name="commercial offer" sheetId="11" r:id="rId10"/>
     <sheet name="negations" sheetId="10" r:id="rId11"/>
+    <sheet name="hints difficulty" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="398">
   <si>
     <t>text</t>
   </si>
@@ -143,9 +144,6 @@
     <t>worth a read</t>
   </si>
   <si>
-    <t>RT @vaughanbell: Scorching response to DSM-5 from ex-chairman Allen Frances is.gd/poqvcs Worth a read - via @psychepi</t>
-  </si>
-  <si>
     <t>scorching response to</t>
   </si>
   <si>
@@ -227,9 +225,6 @@
     <t>congrats to</t>
   </si>
   <si>
-    <t>Just to clarify, of course congrats to all who participated - it's a demanding task - but many demonstrated focus on technical novelty (1/2)</t>
-  </si>
-  <si>
     <t>just finished</t>
   </si>
   <si>
@@ -242,9 +237,6 @@
     <t>Many of the latest job offers atoffice.snd.org/jobs/jobs.lasso are related to #infographics and#dataviz</t>
   </si>
   <si>
-    <t>Businessman goes baaaad. Great piece: NYTimes: John McAfee Plays Hide-and-Seek in Belize</t>
-  </si>
-  <si>
     <t>really</t>
   </si>
   <si>
@@ -269,9 +261,6 @@
     <t>nice</t>
   </si>
   <si>
-    <t>WOW! Impressive!! RT @jasondavies: Geographic polygon clipping: jasondavies.com/maps/clip/ #d3js</t>
-  </si>
-  <si>
     <t>end of sentence and / or immediately preceded by a negative / positive opinion</t>
   </si>
   <si>
@@ -347,9 +336,6 @@
     <t>is a livesaver</t>
   </si>
   <si>
-    <t>japanese green tea is a lifesaver in this condition @cgrltz</t>
-  </si>
-  <si>
     <t>spotlight:</t>
   </si>
   <si>
@@ -446,12 +432,6 @@
     <t>my</t>
   </si>
   <si>
-    <t xml:space="preserve">i love </t>
-  </si>
-  <si>
-    <t>i liked</t>
-  </si>
-  <si>
     <t>enjoy!</t>
   </si>
   <si>
@@ -464,9 +444,6 @@
     <t>impressive</t>
   </si>
   <si>
-    <t>i am so happy</t>
-  </si>
-  <si>
     <t>cool</t>
   </si>
   <si>
@@ -479,21 +456,6 @@
     <t>brilliant</t>
   </si>
   <si>
-    <t>love it</t>
-  </si>
-  <si>
-    <t>i'm happy</t>
-  </si>
-  <si>
-    <t>i am happy</t>
-  </si>
-  <si>
-    <t>i am very happy</t>
-  </si>
-  <si>
-    <t>i'm very happy</t>
-  </si>
-  <si>
     <t>we're honored</t>
   </si>
   <si>
@@ -608,9 +570,6 @@
     <t>have you</t>
   </si>
   <si>
-    <t>get a #FREE</t>
-  </si>
-  <si>
     <t>get a free</t>
   </si>
   <si>
@@ -662,9 +621,6 @@
     <t>desperate</t>
   </si>
   <si>
-    <t>get #free</t>
-  </si>
-  <si>
     <t>not an</t>
   </si>
   <si>
@@ -948,6 +904,321 @@
   </si>
   <si>
     <t>ideas?</t>
+  </si>
+  <si>
+    <t>wait</t>
+  </si>
+  <si>
+    <t>isFirtTermOfStatus,isQuestionMarkAtEndOfStatus</t>
+  </si>
+  <si>
+    <t>meet the new</t>
+  </si>
+  <si>
+    <t>meet</t>
+  </si>
+  <si>
+    <t>dodgy</t>
+  </si>
+  <si>
+    <t>celebrate</t>
+  </si>
+  <si>
+    <t>toxic</t>
+  </si>
+  <si>
+    <t>brand new</t>
+  </si>
+  <si>
+    <t>is out!</t>
+  </si>
+  <si>
+    <t>welcome</t>
+  </si>
+  <si>
+    <t>you're</t>
+  </si>
+  <si>
+    <t>you've</t>
+  </si>
+  <si>
+    <t>aww</t>
+  </si>
+  <si>
+    <t>awww</t>
+  </si>
+  <si>
+    <t>awwww</t>
+  </si>
+  <si>
+    <t>so</t>
+  </si>
+  <si>
+    <t>introducing the</t>
+  </si>
+  <si>
+    <t>should</t>
+  </si>
+  <si>
+    <t>speaking live</t>
+  </si>
+  <si>
+    <t>now only if</t>
+  </si>
+  <si>
+    <t>if only</t>
+  </si>
+  <si>
+    <t>smart</t>
+  </si>
+  <si>
+    <t>cohesive</t>
+  </si>
+  <si>
+    <t>save up to</t>
+  </si>
+  <si>
+    <t>among the top</t>
+  </si>
+  <si>
+    <t>new enhancements</t>
+  </si>
+  <si>
+    <t>new enhancement</t>
+  </si>
+  <si>
+    <t>worst</t>
+  </si>
+  <si>
+    <t>passing the buck</t>
+  </si>
+  <si>
+    <t>passed the buck</t>
+  </si>
+  <si>
+    <t>is like</t>
+  </si>
+  <si>
+    <t>Following @HP 's twitter feed is like observing the captain of the Titanic the month before its first voyage. #HP #Envy #H8</t>
+  </si>
+  <si>
+    <t>introducing</t>
+  </si>
+  <si>
+    <t>strange</t>
+  </si>
+  <si>
+    <t>, right?</t>
+  </si>
+  <si>
+    <t>tweet: And, yah know, being in a distance education program wouldn't require a functioning laptop or anything, right? @HP @HP_support</t>
+  </si>
+  <si>
+    <t>is up</t>
+  </si>
+  <si>
+    <t>merry</t>
+  </si>
+  <si>
+    <t>thank you</t>
+  </si>
+  <si>
+    <t>thx</t>
+  </si>
+  <si>
+    <t>outraged</t>
+  </si>
+  <si>
+    <t>starts with and,</t>
+  </si>
+  <si>
+    <t>starts with or,</t>
+  </si>
+  <si>
+    <t>yah know</t>
+  </si>
+  <si>
+    <t>#free</t>
+  </si>
+  <si>
+    <t>vote now</t>
+  </si>
+  <si>
+    <t>suck</t>
+  </si>
+  <si>
+    <t>lame</t>
+  </si>
+  <si>
+    <t>incredibly</t>
+  </si>
+  <si>
+    <t>IsNotAllCaps</t>
+  </si>
+  <si>
+    <t>never</t>
+  </si>
+  <si>
+    <t>leg up</t>
+  </si>
+  <si>
+    <t>big</t>
+  </si>
+  <si>
+    <t>doubt it</t>
+  </si>
+  <si>
+    <t>never again</t>
+  </si>
+  <si>
+    <t>worse</t>
+  </si>
+  <si>
+    <t>positive and negative, and a thank you in it</t>
+  </si>
+  <si>
+    <t>:/</t>
+  </si>
+  <si>
+    <t>nt an</t>
+  </si>
+  <si>
+    <t>nt my</t>
+  </si>
+  <si>
+    <t>nt the</t>
+  </si>
+  <si>
+    <t>disgusting</t>
+  </si>
+  <si>
+    <t>disgusted</t>
+  </si>
+  <si>
+    <t>disappointed</t>
+  </si>
+  <si>
+    <t>fuming</t>
+  </si>
+  <si>
+    <t>crap</t>
+  </si>
+  <si>
+    <t>insane</t>
+  </si>
+  <si>
+    <t>ur</t>
+  </si>
+  <si>
+    <t>hi</t>
+  </si>
+  <si>
+    <t>wasted time</t>
+  </si>
+  <si>
+    <t>waste my time</t>
+  </si>
+  <si>
+    <t>waste our time</t>
+  </si>
+  <si>
+    <t>incompatible</t>
+  </si>
+  <si>
+    <t>always a pleasure</t>
+  </si>
+  <si>
+    <t>now</t>
+  </si>
+  <si>
+    <t>make it happen with</t>
+  </si>
+  <si>
+    <t>sad</t>
+  </si>
+  <si>
+    <t>fails me</t>
+  </si>
+  <si>
+    <t>we're</t>
+  </si>
+  <si>
+    <t>we've</t>
+  </si>
+  <si>
+    <t>I've</t>
+  </si>
+  <si>
+    <t>I'm</t>
+  </si>
+  <si>
+    <t>mess</t>
+  </si>
+  <si>
+    <t>no, no</t>
+  </si>
+  <si>
+    <t>no no</t>
+  </si>
+  <si>
+    <t>gold</t>
+  </si>
+  <si>
+    <t>care about</t>
+  </si>
+  <si>
+    <t>stunningly</t>
+  </si>
+  <si>
+    <t>liked</t>
+  </si>
+  <si>
+    <t>happy</t>
+  </si>
+  <si>
+    <t>whom</t>
+  </si>
+  <si>
+    <t>what</t>
+  </si>
+  <si>
+    <t>isFirstLetterCapitalized,isQuestionMarkAtEndOfStatus</t>
+  </si>
+  <si>
+    <t>gifts ideas</t>
+  </si>
+  <si>
+    <t>gift ideas</t>
+  </si>
+  <si>
+    <t>stunning</t>
+  </si>
+  <si>
+    <t>grossly</t>
+  </si>
+  <si>
+    <t>awful</t>
+  </si>
+  <si>
+    <t>right wing</t>
+  </si>
+  <si>
+    <t>left wing</t>
+  </si>
+  <si>
+    <t>ultra</t>
+  </si>
+  <si>
+    <t>good read</t>
+  </si>
+  <si>
+    <t>apply</t>
+  </si>
+  <si>
+    <t>apply now</t>
+  </si>
+  <si>
+    <t>find out</t>
   </si>
 </sst>
 </file>
@@ -1303,36 +1574,36 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="120" x14ac:dyDescent="0.25">
@@ -1373,10 +1644,10 @@
         <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1386,10 +1657,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1408,95 +1679,113 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>212</v>
+        <v>337</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>194</v>
-      </c>
+        <v>169</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>195</v>
+      <c r="A6" t="s">
+        <v>228</v>
+      </c>
+      <c r="B6" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="A7" t="s">
+        <v>230</v>
+      </c>
+      <c r="B7" t="s">
+        <v>229</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>243</v>
-      </c>
-      <c r="B8" t="s">
-        <v>244</v>
+        <v>231</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>245</v>
-      </c>
-      <c r="B9" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>246</v>
+        <v>231</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>247</v>
+        <v>233</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>246</v>
+        <v>251</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>248</v>
+        <v>267</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>266</v>
+        <v>278</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>293</v>
+        <v>309</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>299</v>
+        <v>316</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>387</v>
       </c>
     </row>
   </sheetData>
@@ -1507,10 +1796,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A18"/>
+  <dimension ref="A1:A23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A20" sqref="A20:C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1520,92 +1809,177 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>196</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>197</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>214</v>
+        <v>199</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>216</v>
+        <v>201</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>217</v>
+        <v>202</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>295</v>
+        <v>280</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>296</v>
+        <v>281</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>353</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="39.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>323</v>
+      </c>
+      <c r="C1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>327</v>
+      </c>
+      <c r="C2" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>350</v>
       </c>
     </row>
   </sheetData>
@@ -1616,10 +1990,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F83"/>
+  <dimension ref="A1:F89"/>
   <sheetViews>
-    <sheetView topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+    <sheetView topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="A90" sqref="A90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1630,284 +2004,281 @@
     <col min="6" max="6" width="75.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>183</v>
-      </c>
       <c r="B32" s="1" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>131</v>
+        <v>77</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>151</v>
+        <v>179</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>205</v>
+        <v>57</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>116</v>
+        <v>56</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>115</v>
+        <v>128</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -1915,314 +2286,368 @@
         <v>130</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>205</v>
+        <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>192</v>
+        <v>112</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>58</v>
+        <v>113</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>205</v>
+        <v>161</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>133</v>
+      <c r="A45" t="s">
+        <v>145</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>205</v>
+        <v>144</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>119</v>
+        <v>143</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>40</v>
+        <v>192</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>117</v>
+        <v>38</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>205</v>
+        <v>137</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>174</v>
+        <v>227</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>158</v>
+      <c r="A52" s="1" t="s">
+        <v>247</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>157</v>
+        <v>248</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>156</v>
+        <v>77</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>206</v>
+        <v>115</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>205</v>
+        <v>175</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>38</v>
+        <v>116</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>205</v>
+        <v>175</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>144</v>
+        <v>117</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>242</v>
+        <v>118</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>205</v>
+        <v>255</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>205</v>
+        <v>256</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>205</v>
+        <v>257</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>188</v>
+        <v>258</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>121</v>
+        <v>260</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>122</v>
+        <v>261</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>123</v>
+        <v>262</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>270</v>
+        <v>263</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>271</v>
+        <v>264</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>272</v>
+        <v>268</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>273</v>
+        <v>269</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>205</v>
+        <v>285</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>279</v>
+        <v>286</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>283</v>
+        <v>298</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>284</v>
+        <v>302</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>291</v>
+        <v>314</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>292</v>
+        <v>315</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>294</v>
+        <v>317</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>300</v>
+        <v>330</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>301</v>
+        <v>331</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>305</v>
+        <v>332</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>244</v>
+        <v>191</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>211</v>
+        <v>344</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -2236,10 +2661,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="A81" sqref="A81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2280,224 +2705,418 @@
     </row>
     <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>222</v>
+        <v>207</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>226</v>
+        <v>211</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>227</v>
+        <v>212</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>228</v>
+        <v>213</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>232</v>
+        <v>217</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>237</v>
+        <v>222</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>238</v>
+        <v>223</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>239</v>
+        <v>224</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>237</v>
+        <v>222</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>303</v>
+      <c r="B44" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>392</v>
       </c>
     </row>
   </sheetData>
@@ -2508,10 +3127,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2532,7 +3151,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>2</v>
@@ -2543,7 +3162,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>6</v>
@@ -2559,7 +3178,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>15</v>
@@ -2567,140 +3186,184 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>228</v>
+        <v>213</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>229</v>
+        <v>214</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>230</v>
+        <v>215</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>304</v>
+        <v>289</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>190</v>
+        <v>177</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>393</v>
       </c>
     </row>
   </sheetData>
@@ -2711,11 +3374,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A30" sqref="A30"/>
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2735,7 +3398,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="D1" t="s">
         <v>19</v>
@@ -2746,10 +3409,10 @@
     </row>
     <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>20</v>
@@ -2791,7 +3454,7 @@
         <v>30</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D5" t="s">
         <v>24</v>
@@ -2813,7 +3476,7 @@
     </row>
     <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="D7" t="s">
         <v>24</v>
@@ -2846,74 +3509,74 @@
     </row>
     <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D10" t="s">
         <v>24</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="D11" t="s">
         <v>24</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D12" t="s">
         <v>24</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D13" t="s">
         <v>24</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B14" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
       <c r="D14" t="s">
         <v>24</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D15" t="s">
         <v>24</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -2921,105 +3584,158 @@
         <v>31</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D16" t="s">
         <v>24</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B17" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
       <c r="D17" t="s">
         <v>24</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D18" t="s">
         <v>24</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D19" t="s">
         <v>24</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>231</v>
+        <v>216</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>250</v>
+        <v>235</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>257</v>
+        <v>242</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>260</v>
+        <v>245</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>325</v>
+      </c>
+      <c r="B37" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>367</v>
       </c>
     </row>
   </sheetData>
@@ -3030,15 +3746,17 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="26.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="12.42578125" style="1" customWidth="1"/>
     <col min="5" max="6" width="26.42578125" style="1" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="52.85546875" style="1" customWidth="1"/>
@@ -3052,7 +3770,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>2</v>
@@ -3060,137 +3778,169 @@
     </row>
     <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="B9" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>249</v>
+        <v>234</v>
       </c>
       <c r="B11" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="B13"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>256</v>
+        <v>241</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>264</v>
+        <v>249</v>
       </c>
       <c r="B15" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B16" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>269</v>
+        <v>254</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>297</v>
+        <v>282</v>
       </c>
       <c r="B19" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>307</v>
+        <v>292</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>385</v>
       </c>
     </row>
   </sheetData>
@@ -3201,10 +3951,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A7" sqref="A7:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3227,7 +3977,7 @@
     </row>
     <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>4</v>
@@ -3235,22 +3985,42 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>240</v>
+        <v>225</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>241</v>
+        <v>226</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>306</v>
+        <v>291</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>374</v>
       </c>
     </row>
   </sheetData>
@@ -3285,7 +4055,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
@@ -3293,7 +4063,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -3304,10 +4074,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3336,7 +4106,7 @@
     </row>
     <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>3</v>
@@ -3344,7 +4114,7 @@
     </row>
     <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>252</v>
+        <v>237</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>3</v>
@@ -3363,7 +4133,7 @@
     </row>
     <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>33</v>
@@ -3371,7 +4141,7 @@
     </row>
     <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>33</v>
@@ -3379,31 +4149,93 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>267</v>
+        <v>252</v>
       </c>
       <c r="B7" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>268</v>
+        <v>253</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>286</v>
+        <v>271</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>256</v>
+        <v>241</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>287</v>
+        <v>272</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>191</v>
+        <v>178</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>241</v>
       </c>
     </row>
   </sheetData>

</xml_diff>